<commit_message>
Mass moving complete...for now.
All of the cards, barring Baofengs at the moment have been moved over successfully.

Of course, I still need to correct some of the bugs present in a few of them. Again though, any card without code has been removed, so...that should be a bit less.
</commit_message>
<xml_diff>
--- a/Set ID 2019.xlsx
+++ b/Set ID 2019.xlsx
@@ -299,7 +299,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -348,15 +348,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -455,8 +451,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C29" activeCellId="0" sqref="C29"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -627,9 +623,7 @@
       <c r="AMJ8" s="5"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="6" t="n">
-        <v>233000315</v>
-      </c>
+      <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6" t="s">
         <v>11</v>
@@ -645,9 +639,7 @@
       <c r="AMJ9" s="5"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="6" t="n">
-        <v>233000315</v>
-      </c>
+      <c r="A10" s="6"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6" t="s">
         <v>12</v>
@@ -663,9 +655,7 @@
       <c r="AMJ10" s="5"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="6" t="n">
-        <v>233000315</v>
-      </c>
+      <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6" t="s">
         <v>13</v>
@@ -681,9 +671,7 @@
       <c r="AMJ11" s="5"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="6" t="n">
-        <v>233000315</v>
-      </c>
+      <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6" t="s">
         <v>14</v>
@@ -812,19 +800,19 @@
       <c r="AMJ18" s="5"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="11" t="n">
+      <c r="A19" s="6" t="n">
         <v>233000600</v>
       </c>
-      <c r="B19" s="11" t="n">
+      <c r="B19" s="6" t="n">
         <v>233000684</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C19" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D19" s="12" t="n">
+      <c r="D19" s="7" t="n">
         <v>1081</v>
       </c>
-      <c r="E19" s="11" t="str">
+      <c r="E19" s="6" t="str">
         <f aca="false">DEC2HEX(D19)</f>
         <v>439</v>
       </c>
@@ -832,17 +820,15 @@
       <c r="AMJ19" s="5"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="11" t="n">
-        <v>233000600</v>
-      </c>
-      <c r="B20" s="11"/>
-      <c r="C20" s="11" t="s">
+      <c r="A20" s="6"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D20" s="11" t="n">
+      <c r="D20" s="6" t="n">
         <v>5177</v>
       </c>
-      <c r="E20" s="11" t="str">
+      <c r="E20" s="6" t="str">
         <f aca="false">DEC2HEX(D20)</f>
         <v>1439</v>
       </c>
@@ -850,17 +836,15 @@
       <c r="AMJ20" s="5"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="11" t="n">
-        <v>233000600</v>
-      </c>
-      <c r="B21" s="11"/>
-      <c r="C21" s="11" t="s">
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D21" s="11" t="n">
+      <c r="D21" s="6" t="n">
         <v>9273</v>
       </c>
-      <c r="E21" s="11" t="str">
+      <c r="E21" s="6" t="str">
         <f aca="false">DEC2HEX(D21)</f>
         <v>2439</v>
       </c>
@@ -868,17 +852,17 @@
       <c r="AMJ21" s="5"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="11" t="n">
+      <c r="A22" s="6" t="n">
         <v>233000685</v>
       </c>
-      <c r="B22" s="11" t="n">
+      <c r="B22" s="6" t="n">
         <v>233000699</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="C22" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
       <c r="AMI22" s="5"/>
       <c r="AMJ22" s="5"/>
     </row>
@@ -960,32 +944,32 @@
       <c r="AMJ26" s="5"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="11" t="n">
+      <c r="A27" s="6" t="n">
         <v>233000900</v>
       </c>
-      <c r="B27" s="11"/>
-      <c r="C27" s="11" t="s">
+      <c r="B27" s="6"/>
+      <c r="C27" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D27" s="11"/>
-      <c r="E27" s="11" t="n">
+      <c r="D27" s="6"/>
+      <c r="E27" s="6" t="n">
         <v>0</v>
       </c>
       <c r="AMI27" s="5"/>
       <c r="AMJ27" s="5"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="11" t="n">
+      <c r="A28" s="6" t="n">
         <v>233001000</v>
       </c>
-      <c r="B28" s="11"/>
-      <c r="C28" s="11" t="s">
+      <c r="B28" s="6"/>
+      <c r="C28" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D28" s="11" t="n">
+      <c r="D28" s="6" t="n">
         <v>1527</v>
       </c>
-      <c r="E28" s="11" t="str">
+      <c r="E28" s="6" t="str">
         <f aca="false">DEC2HEX(D28)</f>
         <v>5F7</v>
       </c>
@@ -993,37 +977,35 @@
       <c r="AMJ28" s="5"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="11" t="n">
-        <v>233001000</v>
-      </c>
-      <c r="B29" s="11"/>
-      <c r="C29" s="11" t="s">
+      <c r="A29" s="6"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D29" s="11" t="n">
+      <c r="D29" s="6" t="n">
         <v>1528</v>
       </c>
-      <c r="E29" s="11" t="str">
+      <c r="E29" s="6" t="str">
         <f aca="false">DEC2HEX(D29)</f>
         <v>5F8</v>
       </c>
-      <c r="I29" s="13"/>
-      <c r="J29" s="13"/>
+      <c r="I29" s="12"/>
+      <c r="J29" s="12"/>
       <c r="AMI29" s="5"/>
       <c r="AMJ29" s="5"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="11" t="n">
+      <c r="A30" s="6" t="n">
         <v>233001061</v>
       </c>
-      <c r="B30" s="11"/>
-      <c r="C30" s="11" t="s">
+      <c r="B30" s="6"/>
+      <c r="C30" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D30" s="11" t="n">
+      <c r="D30" s="6" t="n">
         <v>1529</v>
       </c>
-      <c r="E30" s="11" t="str">
+      <c r="E30" s="6" t="str">
         <f aca="false">DEC2HEX(D30)</f>
         <v>5F9</v>
       </c>
@@ -1031,17 +1013,17 @@
       <c r="AMJ30" s="5"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="11" t="n">
+      <c r="A31" s="6" t="n">
         <v>233001100</v>
       </c>
-      <c r="B31" s="11"/>
-      <c r="C31" s="11" t="s">
+      <c r="B31" s="6"/>
+      <c r="C31" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D31" s="11" t="n">
+      <c r="D31" s="6" t="n">
         <v>2000</v>
       </c>
-      <c r="E31" s="11" t="str">
+      <c r="E31" s="6" t="str">
         <f aca="false">DEC2HEX(D31)</f>
         <v>7D0</v>
       </c>
@@ -1049,17 +1031,17 @@
       <c r="AMJ31" s="5"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="11" t="n">
+      <c r="A32" s="6" t="n">
         <v>233001200</v>
       </c>
-      <c r="B32" s="11"/>
-      <c r="C32" s="12" t="s">
+      <c r="B32" s="6"/>
+      <c r="C32" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D32" s="12" t="n">
+      <c r="D32" s="7" t="n">
         <v>1225</v>
       </c>
-      <c r="E32" s="11" t="str">
+      <c r="E32" s="6" t="str">
         <f aca="false">DEC2HEX(D32)</f>
         <v>4C9</v>
       </c>
@@ -1067,17 +1049,15 @@
       <c r="AMJ32" s="5"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="11" t="n">
-        <v>233001200</v>
-      </c>
-      <c r="B33" s="11"/>
-      <c r="C33" s="11" t="s">
+      <c r="A33" s="6"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D33" s="11" t="n">
+      <c r="D33" s="6" t="n">
         <v>5321</v>
       </c>
-      <c r="E33" s="11" t="str">
+      <c r="E33" s="6" t="str">
         <f aca="false">DEC2HEX(D33)</f>
         <v>14C9</v>
       </c>
@@ -1085,17 +1065,17 @@
       <c r="AMJ33" s="5"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="11" t="n">
+      <c r="A34" s="6" t="n">
         <v>233001200</v>
       </c>
-      <c r="B34" s="11"/>
-      <c r="C34" s="11" t="s">
+      <c r="B34" s="6"/>
+      <c r="C34" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D34" s="11" t="n">
+      <c r="D34" s="6" t="n">
         <v>9417</v>
       </c>
-      <c r="E34" s="11" t="str">
+      <c r="E34" s="6" t="str">
         <f aca="false">DEC2HEX(D34)</f>
         <v>24C9</v>
       </c>
@@ -1103,17 +1083,17 @@
       <c r="AMJ34" s="5"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="11" t="n">
+      <c r="A35" s="6" t="n">
         <v>233001251</v>
       </c>
-      <c r="B35" s="11"/>
-      <c r="C35" s="12" t="s">
+      <c r="B35" s="6"/>
+      <c r="C35" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D35" s="12" t="n">
+      <c r="D35" s="7" t="n">
         <v>2512</v>
       </c>
-      <c r="E35" s="11" t="str">
+      <c r="E35" s="6" t="str">
         <f aca="false">DEC2HEX(D35)</f>
         <v>9D0</v>
       </c>
@@ -1121,17 +1101,15 @@
       <c r="AMJ35" s="5"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="11" t="n">
-        <v>233001251</v>
-      </c>
-      <c r="B36" s="11"/>
-      <c r="C36" s="11" t="s">
+      <c r="A36" s="6"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D36" s="14" t="n">
+      <c r="D36" s="13" t="n">
         <v>2820560</v>
       </c>
-      <c r="E36" s="11" t="str">
+      <c r="E36" s="6" t="str">
         <f aca="false">DEC2HEX(D36)</f>
         <v>2B09D0</v>
       </c>
@@ -1159,19 +1137,19 @@
       <c r="AMJ37" s="5"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="15" t="n">
+      <c r="A38" s="14" t="n">
         <v>233001314</v>
       </c>
-      <c r="B38" s="15" t="n">
+      <c r="B38" s="14" t="n">
         <v>233001327</v>
       </c>
-      <c r="C38" s="15" t="s">
+      <c r="C38" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="D38" s="15" t="n">
+      <c r="D38" s="14" t="n">
         <v>2008</v>
       </c>
-      <c r="E38" s="15" t="str">
+      <c r="E38" s="14" t="str">
         <f aca="false">DEC2HEX(D38)</f>
         <v>7D8</v>
       </c>
@@ -1183,7 +1161,7 @@
       <c r="AMJ39" s="5"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="16"/>
+      <c r="A40" s="15"/>
       <c r="C40" s="1" t="s">
         <v>41</v>
       </c>
@@ -1191,7 +1169,7 @@
       <c r="AMJ40" s="5"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="17"/>
+      <c r="A41" s="16"/>
       <c r="C41" s="1" t="s">
         <v>42</v>
       </c>
@@ -1199,7 +1177,7 @@
       <c r="AMJ41" s="5"/>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="18"/>
+      <c r="A42" s="17"/>
       <c r="C42" s="1" t="s">
         <v>43</v>
       </c>

</xml_diff>